<commit_message>
updating code to run from cl
</commit_message>
<xml_diff>
--- a/data/darkside/rug_herrschners.xlsx
+++ b/data/darkside/rug_herrschners.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1900" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1900" uniqueCount="32">
   <si>
     <t>black</t>
   </si>
@@ -61,7 +61,7 @@
     <t>light-aqua</t>
   </si>
   <si>
-    <t>bright-yellow</t>
+    <t>yellow</t>
   </si>
   <si>
     <t>dark-red</t>
@@ -85,10 +85,10 @@
     <t>coffee</t>
   </si>
   <si>
-    <t>blue-violet</t>
+    <t>bright-yellow</t>
   </si>
   <si>
-    <t>dark-lavender</t>
+    <t>blue-violet</t>
   </si>
   <si>
     <t>bright-red</t>
@@ -98,6 +98,9 @@
   </si>
   <si>
     <t>light-teal</t>
+  </si>
+  <si>
+    <t>dark-lavender</t>
   </si>
   <si>
     <t>terra-cotta</t>
@@ -3444,7 +3447,7 @@
         <v>0</v>
       </c>
       <c r="AB15" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="AC15" t="s">
         <v>0</v>
@@ -4091,7 +4094,7 @@
         <v>22</v>
       </c>
       <c r="AK19" t="s">
-        <v>0</v>
+        <v>22</v>
       </c>
       <c r="AL19" t="s">
         <v>0</v>
@@ -4243,7 +4246,7 @@
         <v>20</v>
       </c>
       <c r="AJ20" t="s">
-        <v>11</v>
+        <v>20</v>
       </c>
       <c r="AK20" t="s">
         <v>11</v>
@@ -4401,10 +4404,10 @@
         <v>12</v>
       </c>
       <c r="AK21" t="s">
-        <v>15</v>
+        <v>23</v>
       </c>
       <c r="AL21" t="s">
-        <v>15</v>
+        <v>23</v>
       </c>
       <c r="AM21" t="s">
         <v>15</v>
@@ -4571,13 +4574,13 @@
         <v>12</v>
       </c>
       <c r="AP22" t="s">
-        <v>15</v>
+        <v>23</v>
       </c>
       <c r="AQ22" t="s">
-        <v>15</v>
+        <v>23</v>
       </c>
       <c r="AR22" t="s">
-        <v>15</v>
+        <v>23</v>
       </c>
       <c r="AS22" t="s">
         <v>17</v>
@@ -4592,7 +4595,7 @@
         <v>20</v>
       </c>
       <c r="AW22" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="AX22" t="s">
         <v>0</v>
@@ -4711,10 +4714,10 @@
         <v>0</v>
       </c>
       <c r="AK23" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="AL23" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="AM23" t="s">
         <v>18</v>
@@ -4741,13 +4744,13 @@
         <v>12</v>
       </c>
       <c r="AU23" t="s">
-        <v>15</v>
+        <v>23</v>
       </c>
       <c r="AV23" t="s">
-        <v>15</v>
+        <v>23</v>
       </c>
       <c r="AW23" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="AX23" t="s">
         <v>0</v>
@@ -4818,7 +4821,7 @@
         <v>0</v>
       </c>
       <c r="U24" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="V24" t="s">
         <v>0</v>
@@ -4878,10 +4881,10 @@
         <v>0</v>
       </c>
       <c r="AO24" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="AP24" t="s">
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="AQ24" t="s">
         <v>18</v>
@@ -4890,7 +4893,7 @@
         <v>26</v>
       </c>
       <c r="AS24" t="s">
-        <v>26</v>
+        <v>14</v>
       </c>
       <c r="AT24" t="s">
         <v>27</v>
@@ -4902,7 +4905,7 @@
         <v>14</v>
       </c>
       <c r="AW24" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="AX24" t="s">
         <v>0</v>

</xml_diff>